<commit_message>
Extraction + Affichage des molécules
</commit_message>
<xml_diff>
--- a/extraction/etape1_pageform.xlsx
+++ b/extraction/etape1_pageform.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Sample Number</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>Col</t>
+  </si>
+  <si>
+    <t>INN</t>
   </si>
   <si>
     <t>10-12</t>
@@ -404,7 +407,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D241"/>
+  <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -412,7 +415,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,3362 +428,3365 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D27">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D33">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D35">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D36">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D37">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D38">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D39">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D40">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D41">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D45">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D46">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D47">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D48">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D49">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D50">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D51">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D52">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D53">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D54">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D55">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D56">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D57">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D58">
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59">
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D60">
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D61">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D62">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D63">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D64">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D65">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D66">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D67">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D68">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D69">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D70">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D71">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D72">
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D73">
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D74">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D75">
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D76">
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D77">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D78">
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D79">
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D80">
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D81">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D82">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D83">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D84">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D85">
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D86">
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D87">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D88">
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D89">
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D90">
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D91">
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D92">
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D93">
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D94">
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D95">
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D96">
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D97">
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D98">
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D99">
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D100">
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D101">
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D102">
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D103">
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D104">
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D105">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D106">
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D107">
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D108">
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D109">
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D110">
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D111">
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D112">
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D113">
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D114">
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D115">
         <v>16</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D116">
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:5">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D117">
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D118">
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D119">
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D120">
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D121">
         <v>22</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D122">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:5">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D123">
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:5">
       <c r="A124">
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D124">
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D125">
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:5">
       <c r="A126">
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D126">
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="A127">
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D127">
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:5">
       <c r="A128">
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D128">
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:5">
       <c r="A129">
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D129">
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:5">
       <c r="A130">
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D130">
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:5">
       <c r="A131">
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D131">
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:5">
       <c r="A132">
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D132">
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:5">
       <c r="A133">
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D133">
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:5">
       <c r="A134">
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D134">
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:5">
       <c r="A135">
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D135">
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:5">
       <c r="A136">
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D136">
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:5">
       <c r="A137">
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D137">
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:5">
       <c r="A138">
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C138" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D138">
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:5">
       <c r="A139">
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C139" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D139">
         <v>20</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D140">
         <v>21</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:5">
       <c r="A141">
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D141">
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:5">
       <c r="A142">
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D142">
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:5">
       <c r="A143">
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C143" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D143">
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:5">
       <c r="A144">
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C144" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D144">
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:5">
       <c r="A145">
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C145" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D145">
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:5">
       <c r="A146">
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D146">
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:5">
       <c r="A147">
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C147" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D147">
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:5">
       <c r="A148">
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C148" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D148">
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:5">
       <c r="A149">
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C149" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D149">
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:5">
       <c r="A150">
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C150" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D150">
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:5">
       <c r="A151">
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C151" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D151">
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:5">
       <c r="A152">
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C152" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D152">
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:5">
       <c r="A153">
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D153">
         <v>14</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:5">
       <c r="A154">
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D154">
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:5">
       <c r="A155">
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D155">
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:5">
       <c r="A156">
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D156">
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:5">
       <c r="A157">
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D157">
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:5">
       <c r="A158">
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D158">
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:5">
       <c r="A159">
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D159">
         <v>20</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:5">
       <c r="A160">
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C160" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D160">
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:5">
       <c r="A161">
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D161">
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:5">
       <c r="A162">
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D162">
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:5">
       <c r="A163">
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D163">
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:5">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D164">
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:5">
       <c r="A165">
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D165">
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:5">
       <c r="A166">
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D166">
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:5">
       <c r="A167">
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D167">
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:5">
       <c r="A168">
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D168">
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:5">
       <c r="A169">
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D169">
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:5">
       <c r="A170">
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D170">
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:5">
       <c r="A171">
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D171">
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:5">
       <c r="A172">
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D172">
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:5">
       <c r="A173">
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D173">
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:5">
       <c r="A174">
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D174">
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:5">
       <c r="A175">
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D175">
         <v>16</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:5">
       <c r="A176">
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D176">
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:5">
       <c r="A177">
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D177">
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:5">
       <c r="A178">
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D178">
         <v>19</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:5">
       <c r="A179">
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D179">
         <v>20</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:5">
       <c r="A180">
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D180">
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:5">
       <c r="A181">
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D181">
         <v>22</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:5">
       <c r="A182">
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C182" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D182">
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:5">
       <c r="A183">
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D183">
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:5">
       <c r="A184">
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C184" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D184">
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:5">
       <c r="A185">
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C185" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D185">
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:5">
       <c r="A186">
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C186" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D186">
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:5">
       <c r="A187">
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D187">
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:5">
       <c r="A188">
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D188">
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:5">
       <c r="A189">
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C189" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D189">
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:5">
       <c r="A190">
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C190" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D190">
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:5">
       <c r="A191">
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C191" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D191">
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:5">
       <c r="A192">
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C192" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D192">
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:5">
       <c r="A193">
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C193" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D193">
         <v>14</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:5">
       <c r="A194">
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C194" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D194">
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:5">
       <c r="A195">
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C195" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D195">
         <v>16</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:5">
       <c r="A196">
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C196" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D196">
         <v>17</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:5">
       <c r="A197">
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C197" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D197">
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:5">
       <c r="A198">
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C198" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D198">
         <v>19</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:5">
       <c r="A199">
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C199" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D199">
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:5">
       <c r="A200">
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C200" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D200">
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:5">
       <c r="A201">
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D201">
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:5">
       <c r="A202">
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C202" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D202">
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:5">
       <c r="A203">
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C203" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D203">
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:4">
+    <row r="204" spans="1:5">
       <c r="A204">
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C204" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D204">
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:5">
       <c r="A205">
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C205" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D205">
         <v>6</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:5">
       <c r="A206">
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C206" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D206">
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:5">
       <c r="A207">
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C207" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D207">
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:5">
       <c r="A208">
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C208" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D208">
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:5">
       <c r="A209">
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C209" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D209">
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:5">
       <c r="A210">
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C210" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D210">
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:5">
       <c r="A211">
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D211">
         <v>12</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:5">
       <c r="A212">
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C212" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D212">
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:5">
       <c r="A213">
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C213" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D213">
         <v>14</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:5">
       <c r="A214">
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C214" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D214">
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:5">
       <c r="A215">
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C215" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D215">
         <v>16</v>
       </c>
     </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:5">
       <c r="A216">
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C216" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D216">
         <v>17</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:5">
       <c r="A217">
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C217" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D217">
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:5">
       <c r="A218">
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C218" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D218">
         <v>19</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:5">
       <c r="A219">
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C219" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D219">
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:5">
       <c r="A220">
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C220" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D220">
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:4">
+    <row r="221" spans="1:5">
       <c r="A221">
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C221" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D221">
         <v>22</v>
       </c>
     </row>
-    <row r="222" spans="1:4">
+    <row r="222" spans="1:5">
       <c r="A222">
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C222" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D222">
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="1:4">
+    <row r="223" spans="1:5">
       <c r="A223">
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C223" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D223">
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:4">
+    <row r="224" spans="1:5">
       <c r="A224">
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C224" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D224">
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:4">
+    <row r="225" spans="1:5">
       <c r="A225">
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C225" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D225">
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:5">
       <c r="A226">
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C226" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D226">
         <v>7</v>
       </c>
     </row>
-    <row r="227" spans="1:4">
+    <row r="227" spans="1:5">
       <c r="A227">
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C227" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D227">
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:4">
+    <row r="228" spans="1:5">
       <c r="A228">
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C228" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D228">
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:4">
+    <row r="229" spans="1:5">
       <c r="A229">
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C229" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D229">
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:5">
       <c r="A230">
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C230" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D230">
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:5">
       <c r="A231">
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C231" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D231">
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:4">
+    <row r="232" spans="1:5">
       <c r="A232">
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C232" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D232">
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:4">
+    <row r="233" spans="1:5">
       <c r="A233">
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C233" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D233">
         <v>14</v>
       </c>
     </row>
-    <row r="234" spans="1:4">
+    <row r="234" spans="1:5">
       <c r="A234">
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C234" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D234">
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:4">
+    <row r="235" spans="1:5">
       <c r="A235">
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C235" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D235">
         <v>16</v>
       </c>
     </row>
-    <row r="236" spans="1:4">
+    <row r="236" spans="1:5">
       <c r="A236">
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C236" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D236">
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:4">
+    <row r="237" spans="1:5">
       <c r="A237">
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C237" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D237">
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:4">
+    <row r="238" spans="1:5">
       <c r="A238">
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D238">
         <v>19</v>
       </c>
     </row>
-    <row r="239" spans="1:4">
+    <row r="239" spans="1:5">
       <c r="A239">
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C239" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D239">
         <v>20</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
+    <row r="240" spans="1:5">
       <c r="A240">
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C240" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D240">
         <v>21</v>
       </c>
     </row>
-    <row r="241" spans="1:4">
+    <row r="241" spans="1:5">
       <c r="A241">
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C241" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D241">
         <v>22</v>

</xml_diff>

<commit_message>
mise a jour extraction
</commit_message>
<xml_diff>
--- a/extraction/etape1_pageform.xlsx
+++ b/extraction/etape1_pageform.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Sample Number</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>CTRL DMSO</t>
   </si>
 </sst>
 </file>
@@ -407,7 +419,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E241"/>
+  <dimension ref="A1:E249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3790,6 +3802,39 @@
       </c>
       <c r="D241">
         <v>22</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="E243" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="E244" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="E245" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="B247" t="s">
+        <v>21</v>
+      </c>
+      <c r="E247" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="E248" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="E249" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>